<commit_message>
changing sizes to 16:9 now
</commit_message>
<xml_diff>
--- a/color-table-data/color-table.xlsx
+++ b/color-table-data/color-table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="color" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,10 +13,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>color</t>
+    <t>DataValue</t>
+  </si>
+  <si>
+    <t>Color</t>
   </si>
   <si>
     <t>Binder</t>
@@ -87,12 +87,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,7 +111,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">

</xml_diff>